<commit_message>
Updated input_util.py to support spreadsheets that define a "titles" column rather than "title"
</commit_message>
<xml_diff>
--- a/src/pds_doi_service/core/input/test/data/spreadsheet_with_malformed_column_names.xlsx
+++ b/src/pds_doi_service/core/input/test/data/spreadsheet_with_malformed_column_names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collinss/repos/pds-doi-service/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collinss/repos/pds-doi-service/src/pds_doi_service/core/input/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E08F391-EBA1-DD4C-B902-BA60877C6EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91700481-FADF-7144-9DDE-D4847C3A5D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5500" yWindow="6300" windowWidth="23300" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Laboratory Shocked Feldspars Bundle</t>
   </si>
   <si>
-    <t xml:space="preserve">   title  </t>
-  </si>
-  <si>
     <t>Publication_date (yyyy-mm-dd)</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   <si>
     <t xml:space="preserve">   related_resource
 LIDVID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   titleS  </t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -412,25 +412,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>